<commit_message>
other roles views added.
</commit_message>
<xml_diff>
--- a/docs/dataDictionary.xlsx
+++ b/docs/dataDictionary.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="DataDictionary" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -149,9 +149,6 @@
     <t>CK phone mask (phone ~ '^\+7[\s()-]*\d{3}[\s()-]*\d{3}[\s()-]*\d{2}[\s()-]*\d{2}$')</t>
   </si>
   <si>
-    <t>CK email mask (email LIKE '%@%._%')</t>
-  </si>
-  <si>
     <t>pass</t>
   </si>
   <si>
@@ -273,6 +270,9 @@
   </si>
   <si>
     <t>FK to jury</t>
+  </si>
+  <si>
+    <t>unique, CK email mask (email LIKE '%@%._%')</t>
   </si>
 </sst>
 </file>
@@ -814,7 +814,7 @@
   <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E80" sqref="E80"/>
+      <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -1265,7 +1265,7 @@
         <v>7</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="53.25" customHeight="1">
@@ -1286,10 +1286,10 @@
     <row r="36" spans="1:5">
       <c r="A36" s="8"/>
       <c r="B36" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="19" t="s">
         <v>45</v>
-      </c>
-      <c r="C36" s="19" t="s">
-        <v>46</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>7</v>
@@ -1302,7 +1302,7 @@
         <v>23</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>7</v>
@@ -1312,19 +1312,19 @@
     <row r="38" spans="1:5" ht="30">
       <c r="A38" s="8"/>
       <c r="B38" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="C38" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="D38" s="8"/>
       <c r="E38" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" s="21"/>
       <c r="C40" s="21"/>
@@ -1350,10 +1350,10 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C42" s="17" t="s">
         <v>20</v>
@@ -1362,15 +1362,15 @@
         <v>7</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>20</v>
@@ -1379,15 +1379,15 @@
         <v>7</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>20</v>
@@ -1396,12 +1396,12 @@
         <v>7</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B46" s="21"/>
       <c r="C46" s="21"/>
@@ -1427,10 +1427,10 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C48" s="17" t="s">
         <v>20</v>
@@ -1439,15 +1439,15 @@
         <v>7</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>20</v>
@@ -1456,7 +1456,7 @@
         <v>7</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1465,7 +1465,7 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B51" s="21"/>
       <c r="C51" s="21"/>
@@ -1509,7 +1509,7 @@
     <row r="54" spans="1:5">
       <c r="A54" s="8"/>
       <c r="B54" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C54" s="17" t="s">
         <v>41</v>
@@ -1522,7 +1522,7 @@
     <row r="55" spans="1:5">
       <c r="A55" s="8"/>
       <c r="B55" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C55" s="19" t="s">
         <v>36</v>
@@ -1535,7 +1535,7 @@
     <row r="56" spans="1:5">
       <c r="A56" s="8"/>
       <c r="B56" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C56" s="19" t="s">
         <v>20</v>
@@ -1544,7 +1544,7 @@
         <v>7</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1552,7 +1552,7 @@
         <v>38</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C57" s="19" t="s">
         <v>20</v>
@@ -1561,7 +1561,7 @@
         <v>7</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1570,14 +1570,14 @@
         <v>23</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D58" s="8"/>
       <c r="E58" s="3"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B60" s="21"/>
       <c r="C60" s="21"/>
@@ -1623,7 +1623,7 @@
         <v>38</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C63" s="17" t="s">
         <v>20</v>
@@ -1632,7 +1632,7 @@
         <v>7</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1640,20 +1640,20 @@
         <v>38</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C64" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D64" s="8"/>
       <c r="E64" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="8"/>
       <c r="B65" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C65" s="19" t="s">
         <v>20</v>
@@ -1662,12 +1662,12 @@
         <v>7</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B67" s="21"/>
       <c r="C67" s="21"/>
@@ -1713,7 +1713,7 @@
         <v>38</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C70" s="17" t="s">
         <v>20</v>
@@ -1722,13 +1722,13 @@
         <v>7</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="8"/>
       <c r="B71" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C71" s="19" t="s">
         <v>25</v>
@@ -1741,7 +1741,7 @@
     <row r="72" spans="1:5">
       <c r="A72" s="8"/>
       <c r="B72" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C72" s="19" t="s">
         <v>20</v>
@@ -1750,16 +1750,16 @@
         <v>7</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="8"/>
       <c r="B73" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C73" s="19" t="s">
         <v>75</v>
-      </c>
-      <c r="C73" s="19" t="s">
-        <v>76</v>
       </c>
       <c r="D73" s="8" t="s">
         <v>7</v>
@@ -1771,19 +1771,19 @@
         <v>38</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C74" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D74" s="8"/>
       <c r="E74" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B76" s="21"/>
       <c r="C76" s="21"/>
@@ -1809,10 +1809,10 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C78" s="17" t="s">
         <v>20</v>
@@ -1821,15 +1821,15 @@
         <v>7</v>
       </c>
       <c r="E78" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C79" s="17" t="s">
         <v>20</v>
@@ -1838,23 +1838,23 @@
         <v>7</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A17:E17"/>
     <mergeCell ref="A76:E76"/>
     <mergeCell ref="A40:E40"/>
     <mergeCell ref="A46:E46"/>
     <mergeCell ref="A51:E51"/>
     <mergeCell ref="A60:E60"/>
     <mergeCell ref="A67:E67"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A17:E17"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.2" right="0.2" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>

</xml_diff>